<commit_message>
fix output of regressions and rebase age group variable
</commit_message>
<xml_diff>
--- a/OUTPUT/DATA/Regression output 2022.xlsx
+++ b/OUTPUT/DATA/Regression output 2022.xlsx
@@ -1,162 +1,218 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://greaterlondonauthority.sharepoint.com/sites/S_IU_GLAEconomics/Shared Documents/General/Micro/Labour Market/Ad hoc work/12. Childcare and employment/R/OUTPUT/DATA/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_B126ED787D37D8BD5361C41F71B3093A3B2761B1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC198EBE-F1B1-4D42-9DC7-7B092FF1602F}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
-  <si>
-    <t xml:space="preserve"/>
-  </si>
-  <si>
-    <t xml:space="preserve">(Intercept)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SEX_labelFemale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">parent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">age_groupAged 18-24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">age_groupAged 25-34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">age_groupAged 35-49</t>
-  </si>
-  <si>
-    <t xml:space="preserve">age_groupAged 50-64</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SEX_labelFemale:parent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SEX_labelFemale:age_groupAged 18-24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SEX_labelFemale:age_groupAged 25-34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SEX_labelFemale:age_groupAged 35-49</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SEX_labelFemale:age_groupAged 50-64</t>
-  </si>
-  <si>
-    <t xml:space="preserve">parent:age_groupAged 18-24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">parent:age_groupAged 25-34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">parent:age_groupAged 35-49</t>
-  </si>
-  <si>
-    <t xml:space="preserve">parent:age_groupAged 50-64</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SEX_labelFemale:parent:age_groupAged 18-24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SEX_labelFemale:parent:age_groupAged 25-34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SEX_labelFemale:parent:age_groupAged 35-49</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SEX_labelFemale:parent:age_groupAged 50-64</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R2</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="62">
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>(Intercept)</t>
+  </si>
+  <si>
+    <t>parent</t>
+  </si>
+  <si>
+    <t>SEX_labelFemale</t>
+  </si>
+  <si>
+    <t>parent:SEX_labelFemale</t>
+  </si>
+  <si>
+    <t>age_groupAged 16-17</t>
+  </si>
+  <si>
+    <t>age_groupAged 18-24</t>
+  </si>
+  <si>
+    <t>age_groupAged 35-49</t>
+  </si>
+  <si>
+    <t>age_groupAged 50-64</t>
+  </si>
+  <si>
+    <t>parent:age_groupAged 16-17</t>
+  </si>
+  <si>
+    <t>parent:age_groupAged 18-24</t>
+  </si>
+  <si>
+    <t>parent:age_groupAged 35-49</t>
+  </si>
+  <si>
+    <t>parent:age_groupAged 50-64</t>
+  </si>
+  <si>
+    <t>SEX_labelFemale:age_groupAged 16-17</t>
+  </si>
+  <si>
+    <t>SEX_labelFemale:age_groupAged 18-24</t>
+  </si>
+  <si>
+    <t>SEX_labelFemale:age_groupAged 35-49</t>
+  </si>
+  <si>
+    <t>SEX_labelFemale:age_groupAged 50-64</t>
+  </si>
+  <si>
+    <t>parent:SEX_labelFemale:age_groupAged 16-17</t>
+  </si>
+  <si>
+    <t>parent:SEX_labelFemale:age_groupAged 18-24</t>
+  </si>
+  <si>
+    <t>parent:SEX_labelFemale:age_groupAged 35-49</t>
+  </si>
+  <si>
+    <t>parent:SEX_labelFemale:age_groupAged 50-64</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>R2</t>
   </si>
   <si>
     <t xml:space="preserve"> *** p &lt; 0.001;  ** p &lt; 0.01;  * p &lt; 0.05.</t>
   </si>
   <si>
-    <t xml:space="preserve">Model 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.20 ***</t>
+    <t>simple</t>
+  </si>
+  <si>
+    <t>0.71 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.00)   </t>
+  </si>
+  <si>
+    <t>0.12 ***</t>
   </si>
   <si>
     <t xml:space="preserve">(0.01)   </t>
   </si>
   <si>
-    <t xml:space="preserve">0.05 *  </t>
+    <t xml:space="preserve">       </t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>0.75 ***</t>
+  </si>
+  <si>
+    <t>0.13 ***</t>
+  </si>
+  <si>
+    <t>-0.08 ***</t>
+  </si>
+  <si>
+    <t>sex full</t>
+  </si>
+  <si>
+    <t>0.72 ***</t>
+  </si>
+  <si>
+    <t>0.21 ***</t>
+  </si>
+  <si>
+    <t>-0.03 ***</t>
+  </si>
+  <si>
+    <t>-0.15 ***</t>
+  </si>
+  <si>
+    <t>sex &amp; age</t>
+  </si>
+  <si>
+    <t>0.86 ***</t>
+  </si>
+  <si>
+    <t>0.03 ***</t>
+  </si>
+  <si>
+    <t>-0.07 ***</t>
+  </si>
+  <si>
+    <t>-0.60 ***</t>
+  </si>
+  <si>
+    <t>-0.22 ***</t>
+  </si>
+  <si>
+    <t>-0.12 ***</t>
+  </si>
+  <si>
+    <t>sex &amp; age full</t>
+  </si>
+  <si>
+    <t>0.85 ***</t>
+  </si>
+  <si>
+    <t>0.08 ***</t>
+  </si>
+  <si>
+    <t>0.04 ***</t>
+  </si>
+  <si>
+    <t>-0.29 ***</t>
   </si>
   <si>
     <t xml:space="preserve">(0.02)   </t>
   </si>
   <si>
-    <t xml:space="preserve">-0.20 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.39 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.65 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.51 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.05 *  </t>
+    <t>-0.65 ***</t>
+  </si>
+  <si>
+    <t>-0.26 ***</t>
+  </si>
+  <si>
+    <t>-0.14 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.08)   </t>
+  </si>
+  <si>
+    <t>0.11 ***</t>
   </si>
   <si>
     <t xml:space="preserve">(0.03)   </t>
   </si>
   <si>
-    <t xml:space="preserve">-0.07 *  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.11 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.41 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.08)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.29 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.28 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.27 ** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.24 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.08 ** </t>
+    <t>-0.06 ***</t>
+  </si>
+  <si>
+    <t>-0.10 ***</t>
+  </si>
+  <si>
+    <t>0.24 ***</t>
+  </si>
+  <si>
+    <t>0.16 ***</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
-    <numFmt numFmtId="166" formatCode="0.00"/>
-    <numFmt numFmtId="167" formatCode="0.00"/>
-    <numFmt numFmtId="168" formatCode="0.00"/>
-    <numFmt numFmtId="169" formatCode="0.00"/>
-  </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -187,88 +243,58 @@
       <diagonal/>
     </border>
     <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="hair">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
+      <left/>
+      <right/>
       <top style="hair">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="hair">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -277,40 +303,49 @@
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="0" horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="0" horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="0" horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="0" horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="0" horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="0" horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="0" horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="0" horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="0" horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="0" horizontal="right" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -592,379 +627,918 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.71" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="10.71" hidden="0" customWidth="1"/>
+    <col min="1" max="1" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="NA" customHeight="1">
+    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" ht="NA" customHeight="1">
+      <c r="C1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" ht="NA" customHeight="1">
+      <c r="C2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" ht="NA" customHeight="1">
+      <c r="C3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" ht="NA" customHeight="1">
+      <c r="C4" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="6" ht="NA" customHeight="1">
+      <c r="C5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" ht="NA" customHeight="1">
+      <c r="B6" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" ht="NA" customHeight="1">
+      <c r="D7" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" ht="NA" customHeight="1">
+      <c r="B8" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="10" ht="NA" customHeight="1">
+      <c r="E9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" ht="NA" customHeight="1">
+      <c r="B10" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="12" ht="NA" customHeight="1">
+      <c r="F11" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" ht="NA" customHeight="1">
+      <c r="B12" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="14" ht="NA" customHeight="1">
+      <c r="F13" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" ht="NA" customHeight="1">
+      <c r="B14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="F14" s="6">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="16" ht="NA" customHeight="1">
+      <c r="F15" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" ht="NA" customHeight="1">
+      <c r="B16" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="18" ht="NA" customHeight="1">
+      <c r="F17" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="7" t="n">
-        <v>-0.02</v>
-      </c>
-    </row>
-    <row r="19" ht="NA" customHeight="1">
+      <c r="B18" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" ht="NA" customHeight="1">
+      <c r="B19" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="7" t="n">
-        <v>-0.01</v>
-      </c>
-    </row>
-    <row r="21" ht="NA" customHeight="1">
+      <c r="B20" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="6">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B21" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" ht="NA" customHeight="1">
+      <c r="B21" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" ht="NA" customHeight="1">
+      <c r="B22" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="24" ht="NA" customHeight="1">
+      <c r="B23" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" ht="NA" customHeight="1">
+      <c r="B24" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B25" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" ht="NA" customHeight="1">
+      <c r="B25" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="27" ht="NA" customHeight="1">
+      <c r="B26" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F26" s="6">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="28" ht="NA" customHeight="1">
+      <c r="B27" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B28" s="7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="29" ht="NA" customHeight="1">
+      <c r="B28" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F28" s="6">
+        <v>-0.02</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B29" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" ht="NA" customHeight="1">
+      <c r="B29" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="31" ht="NA" customHeight="1">
+      <c r="B30" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B31" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="32" ht="NA" customHeight="1">
+      <c r="B31" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B32" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" ht="NA" customHeight="1">
+      <c r="B32" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F33" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="34" ht="NA" customHeight="1">
+    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="35" ht="NA" customHeight="1">
+      <c r="B34" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B35" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="36" ht="NA" customHeight="1">
+      <c r="B35" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B36" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="37" ht="NA" customHeight="1">
+      <c r="B36" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F36" s="6">
+        <v>-0.03</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B37" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="38" ht="NA" customHeight="1">
+      <c r="B37" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B38" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="39" ht="NA" customHeight="1">
+      <c r="B38" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B39" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="40" ht="NA" customHeight="1">
+      <c r="B39" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B40" s="7" t="n">
-        <v>-0.03</v>
-      </c>
-    </row>
-    <row r="41" ht="NA" customHeight="1">
+      <c r="B40" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B41" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="42" ht="NA" customHeight="1">
+      <c r="B41" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B42" s="9" t="n">
+      <c r="B42" s="8">
         <v>47330</v>
       </c>
-    </row>
-    <row r="43" ht="NA" customHeight="1">
+      <c r="C42" s="8">
+        <v>47330</v>
+      </c>
+      <c r="D42" s="8">
+        <v>47330</v>
+      </c>
+      <c r="E42" s="8">
+        <v>47330</v>
+      </c>
+      <c r="F42" s="8">
+        <v>47330</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B43" s="10" t="n">
+      <c r="B43" s="9">
+        <v>0.02</v>
+      </c>
+      <c r="C43" s="9">
+        <v>0.03</v>
+      </c>
+      <c r="D43" s="9">
+        <v>0.03</v>
+      </c>
+      <c r="E43" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="F43" s="9">
         <v>0.12</v>
       </c>
     </row>
-    <row r="44" ht="NA" customHeight="1">
-      <c r="A44" s="4" t="s">
+    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F44" s="10" t="s">
         <v>23</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A44:F44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100535EDF9DD8DBB143AE8CD71BDB6B0E3B" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="58db4c0cb4a6c8574584e2b7e3b481f7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7fc9ebc1-6786-4aad-aee1-fdcde6e01ff9" xmlns:ns3="fd7425d0-09b7-49b7-b351-1ad2162dc0d7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7f205f5aa0458c3a5f4d8c0367cd4bd4" ns2:_="" ns3:_="">
     <xsd:import namespace="7fc9ebc1-6786-4aad-aee1-fdcde6e01ff9"/>
@@ -1207,34 +1781,29 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7fc9ebc1-6786-4aad-aee1-fdcde6e01ff9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="fd7425d0-09b7-49b7-b351-1ad2162dc0d7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAE230CE-8EAA-48CD-9D36-8E60185CE33A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D33AF8B-2853-4BAD-ACF7-DE7668FAFC68}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8483E32F-E249-488B-A6FD-9F556A02AAC7}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBCFDD39-86D4-4749-A890-DED19F2B4646}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B05076EF-80BF-4908-8FF6-2571E6DF3E9D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="7fc9ebc1-6786-4aad-aee1-fdcde6e01ff9"/>
+    <ds:schemaRef ds:uri="fd7425d0-09b7-49b7-b351-1ad2162dc0d7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
create additional loop layer for UK totals to avoid memory issues; create new output for WFH rates
</commit_message>
<xml_diff>
--- a/OUTPUT/DATA/Regression output 2022.xlsx
+++ b/OUTPUT/DATA/Regression output 2022.xlsx
@@ -1824,22 +1824,22 @@
         <v>25</v>
       </c>
       <c r="B50" s="9" t="n">
-        <v>94660</v>
+        <v>47330</v>
       </c>
       <c r="C50" s="9" t="n">
-        <v>94660</v>
+        <v>47330</v>
       </c>
       <c r="D50" s="9" t="n">
-        <v>94660</v>
+        <v>47330</v>
       </c>
       <c r="E50" s="9" t="n">
-        <v>94660</v>
+        <v>47330</v>
       </c>
       <c r="F50" s="9" t="n">
-        <v>94660</v>
+        <v>47330</v>
       </c>
       <c r="G50" s="9" t="n">
-        <v>94660</v>
+        <v>47330</v>
       </c>
     </row>
     <row r="51" ht="NA" customHeight="1">
@@ -2150,9 +2150,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34DF1716-5AEA-4391-BBC3-930BF388F9CD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC8E39F2-BD0F-45E5-8FA2-97930B5E71AC}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BB10501-302B-4B3F-A0E0-F5CB09CB149A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E84F862-D9C7-4684-B90F-6F1244045D82}"/>
 </file>
</xml_diff>

<commit_message>
begin charting script; add model with child age; trim other models for memory reasons
</commit_message>
<xml_diff>
--- a/OUTPUT/DATA/Regression output 2022.xlsx
+++ b/OUTPUT/DATA/Regression output 2022.xlsx
@@ -2150,9 +2150,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC8E39F2-BD0F-45E5-8FA2-97930B5E71AC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A823A323-2463-413D-BE72-12ED5833C815}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E84F862-D9C7-4684-B90F-6F1244045D82}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{752E60B3-1CB0-4D94-A097-9BFADA9BF35C}"/>
 </file>
</xml_diff>

<commit_message>
add slides to ppt
</commit_message>
<xml_diff>
--- a/OUTPUT/DATA/Regression output 2022.xlsx
+++ b/OUTPUT/DATA/Regression output 2022.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t xml:space="preserve"/>
   </si>
@@ -23,6 +23,9 @@
     <t xml:space="preserve">parent</t>
   </si>
   <si>
+    <t xml:space="preserve">london_resident</t>
+  </si>
+  <si>
     <t xml:space="preserve">SEX_labelFemale</t>
   </si>
   <si>
@@ -53,49 +56,22 @@
     <t xml:space="preserve">age_groupAged 50-64</t>
   </si>
   <si>
-    <t xml:space="preserve">parent:age_groupAged 16-17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">parent:age_groupAged 18-24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">parent:age_groupAged 35-49</t>
-  </si>
-  <si>
-    <t xml:space="preserve">parent:age_groupAged 50-64</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SEX_labelFemale:age_groupAged 16-17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SEX_labelFemale:age_groupAged 18-24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SEX_labelFemale:age_groupAged 35-49</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SEX_labelFemale:age_groupAged 50-64</t>
-  </si>
-  <si>
-    <t xml:space="preserve">parent:SEX_labelFemale:age_groupAged 16-17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">parent:SEX_labelFemale:age_groupAged 18-24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">parent:SEX_labelFemale:age_groupAged 35-49</t>
-  </si>
-  <si>
-    <t xml:space="preserve">parent:SEX_labelFemale:age_groupAged 50-64</t>
-  </si>
-  <si>
     <t xml:space="preserve">age_child3-4 yrs</t>
   </si>
   <si>
     <t xml:space="preserve">age_childMore then 4 yrs</t>
   </si>
   <si>
-    <t xml:space="preserve">ethnicityWhite</t>
+    <t xml:space="preserve">ethnicityBAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parent:ethnicityBAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEX_labelFemale:ethnicityBAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parent:SEX_labelFemale:ethnicityBAME</t>
   </si>
   <si>
     <t xml:space="preserve">N</t>
@@ -140,7 +116,7 @@
     <t xml:space="preserve">famtype</t>
   </si>
   <si>
-    <t xml:space="preserve">0.68 ***</t>
+    <t xml:space="preserve">0.69 ***</t>
   </si>
   <si>
     <t xml:space="preserve">0.42 ***</t>
@@ -176,103 +152,73 @@
     <t xml:space="preserve">sex &amp; age</t>
   </si>
   <si>
-    <t xml:space="preserve">0.86 ***</t>
+    <t xml:space="preserve">0.87 ***</t>
   </si>
   <si>
     <t xml:space="preserve">0.03 ***</t>
   </si>
   <si>
+    <t xml:space="preserve">-0.02 *  </t>
+  </si>
+  <si>
     <t xml:space="preserve">-0.07 ***</t>
   </si>
   <si>
     <t xml:space="preserve">-0.60 ***</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.22 ***</t>
+    <t xml:space="preserve">-0.23 ***</t>
   </si>
   <si>
     <t xml:space="preserve">-0.12 ***</t>
   </si>
   <si>
-    <t xml:space="preserve">sex &amp; age full</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.85 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.08 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.04 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.29 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.65 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.26 ***</t>
+    <t xml:space="preserve">sex &amp; age_child</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.67 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.23 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.06 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sex, eth, age, &amp; age_child</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.80 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.14 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.02 ** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.17 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.62 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.07 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.10 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">full model</t>
   </si>
   <si>
     <t xml:space="preserve">-0.14 ***</t>
   </si>
   <si>
-    <t xml:space="preserve">(0.08)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.11 ***</t>
+    <t xml:space="preserve">-0.06 ***</t>
   </si>
   <si>
     <t xml:space="preserve">(0.03)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.06 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.10 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.24 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.16 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sex &amp; age_child</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.66 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.23 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.06 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sex, eth, age, &amp; age_child</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.14 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.02 ** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.17 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.62 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.23 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.07 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.09 ***</t>
   </si>
 </sst>
 </file>
@@ -744,28 +690,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="H1" s="5" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" ht="NA" customHeight="1">
@@ -773,28 +719,28 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="F2" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>61</v>
-      </c>
       <c r="H2" s="6" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" ht="NA" customHeight="1">
@@ -802,28 +748,28 @@
         <v>0</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" ht="NA" customHeight="1">
@@ -831,28 +777,28 @@
         <v>2</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="F4" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>62</v>
-      </c>
       <c r="H4" s="7" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" ht="NA" customHeight="1">
@@ -860,57 +806,57 @@
         <v>0</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" ht="NA" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>51</v>
+      <c r="B6" s="7" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="C6" s="7" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="D6" s="7" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="E6" s="7" t="n">
+        <v>-0.01</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>81</v>
+        <v>48</v>
+      </c>
+      <c r="G6" s="7" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="H6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="7" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="7" ht="NA" customHeight="1">
@@ -918,28 +864,28 @@
         <v>0</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" ht="NA" customHeight="1">
@@ -947,28 +893,28 @@
         <v>4</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>36</v>
+        <v>60</v>
+      </c>
+      <c r="I8" s="7" t="n">
+        <v>-0.01</v>
       </c>
     </row>
     <row r="9" ht="NA" customHeight="1">
@@ -976,28 +922,28 @@
         <v>0</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" ht="NA" customHeight="1">
@@ -1005,28 +951,28 @@
         <v>5</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>34</v>
-      </c>
       <c r="E10" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" ht="NA" customHeight="1">
@@ -1034,28 +980,28 @@
         <v>0</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" ht="NA" customHeight="1">
@@ -1063,28 +1009,28 @@
         <v>6</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" ht="NA" customHeight="1">
@@ -1092,28 +1038,28 @@
         <v>0</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" ht="NA" customHeight="1">
@@ -1121,28 +1067,28 @@
         <v>7</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" ht="NA" customHeight="1">
@@ -1150,28 +1096,28 @@
         <v>0</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" ht="NA" customHeight="1">
@@ -1179,28 +1125,28 @@
         <v>8</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>82</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" ht="NA" customHeight="1">
@@ -1208,28 +1154,28 @@
         <v>0</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" ht="NA" customHeight="1">
@@ -1237,28 +1183,28 @@
         <v>9</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" ht="NA" customHeight="1">
@@ -1266,28 +1212,28 @@
         <v>0</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" ht="NA" customHeight="1">
@@ -1295,28 +1241,28 @@
         <v>10</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>66</v>
+        <v>28</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" ht="NA" customHeight="1">
@@ -1324,28 +1270,28 @@
         <v>0</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" ht="NA" customHeight="1">
@@ -1353,28 +1299,28 @@
         <v>11</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F22" s="7" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="G22" s="7" t="n">
-        <v>0.01</v>
+        <v>28</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="I22" s="7" t="n">
-        <v>-0.01</v>
+        <v>51</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="23" ht="NA" customHeight="1">
@@ -1382,28 +1328,28 @@
         <v>0</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" ht="NA" customHeight="1">
@@ -1411,28 +1357,28 @@
         <v>12</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>59</v>
+        <v>28</v>
+      </c>
+      <c r="F24" s="7" t="n">
+        <v>0.01</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="H24" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="I24" s="7" t="s">
-        <v>52</v>
+        <v>28</v>
+      </c>
+      <c r="H24" s="7" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="I24" s="7" t="n">
+        <v>-0.01</v>
       </c>
     </row>
     <row r="25" ht="NA" customHeight="1">
@@ -1440,28 +1386,28 @@
         <v>0</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" ht="NA" customHeight="1">
@@ -1469,28 +1415,28 @@
         <v>13</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" ht="NA" customHeight="1">
@@ -1498,28 +1444,28 @@
         <v>0</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" ht="NA" customHeight="1">
@@ -1527,28 +1473,28 @@
         <v>14</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G28" s="7" t="n">
-        <v>0.12</v>
-      </c>
-      <c r="H28" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="I28" s="7" t="s">
-        <v>36</v>
+        <v>-0.01</v>
+      </c>
+      <c r="H28" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" s="7" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="29" ht="NA" customHeight="1">
@@ -1556,28 +1502,28 @@
         <v>0</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>68</v>
+        <v>27</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" ht="NA" customHeight="1">
@@ -1585,28 +1531,28 @@
         <v>15</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G30" s="7" t="n">
-        <v>0</v>
+        <v>28</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>56</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" ht="NA" customHeight="1">
@@ -1614,28 +1560,28 @@
         <v>0</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" ht="NA" customHeight="1">
@@ -1643,28 +1589,28 @@
         <v>16</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>69</v>
+        <v>28</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" ht="NA" customHeight="1">
@@ -1672,28 +1618,28 @@
         <v>0</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" ht="NA" customHeight="1">
@@ -1701,28 +1647,28 @@
         <v>17</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G34" s="7" t="n">
-        <v>0.01</v>
+        <v>28</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="I34" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
+      </c>
+      <c r="I34" s="7" t="n">
+        <v>0.03</v>
       </c>
     </row>
     <row r="35" ht="NA" customHeight="1">
@@ -1730,28 +1676,28 @@
         <v>0</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>70</v>
+        <v>28</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" ht="NA" customHeight="1">
@@ -1759,28 +1705,28 @@
         <v>18</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G36" s="7" t="n">
-        <v>-0.02</v>
+        <v>28</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="I36" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
+      </c>
+      <c r="I36" s="7" t="n">
+        <v>-0.04</v>
       </c>
     </row>
     <row r="37" ht="NA" customHeight="1">
@@ -1788,28 +1734,28 @@
         <v>0</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="38" ht="NA" customHeight="1">
@@ -1817,613 +1763,149 @@
         <v>19</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>71</v>
+        <v>28</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="I38" s="7" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" ht="NA" customHeight="1">
       <c r="A39" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B39" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G39" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="H39" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="I39" s="7" t="s">
-        <v>36</v>
+      <c r="B39" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G39" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H39" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I39" s="8" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="40" ht="NA" customHeight="1">
       <c r="A40" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B40" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F40" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G40" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="H40" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="I40" s="7" t="s">
-        <v>36</v>
+      <c r="B40" s="9" t="n">
+        <v>47330</v>
+      </c>
+      <c r="C40" s="9" t="n">
+        <v>47330</v>
+      </c>
+      <c r="D40" s="9" t="n">
+        <v>47330</v>
+      </c>
+      <c r="E40" s="9" t="n">
+        <v>47330</v>
+      </c>
+      <c r="F40" s="9" t="n">
+        <v>47330</v>
+      </c>
+      <c r="G40" s="9" t="n">
+        <v>47330</v>
+      </c>
+      <c r="H40" s="9" t="n">
+        <v>45146</v>
+      </c>
+      <c r="I40" s="9" t="n">
+        <v>45146</v>
       </c>
     </row>
     <row r="41" ht="NA" customHeight="1">
-      <c r="A41" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G41" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="H41" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="I41" s="7" t="s">
-        <v>36</v>
+      <c r="A41" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" s="10" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="C41" s="10" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="D41" s="10" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="E41" s="10" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="F41" s="10" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G41" s="10" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="H41" s="10" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="I41" s="10" t="n">
+        <v>0.12</v>
       </c>
     </row>
     <row r="42" ht="NA" customHeight="1">
-      <c r="A42" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F42" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G42" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="H42" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="I42" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="43" ht="NA" customHeight="1">
-      <c r="A43" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G43" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="H43" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="I43" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="44" ht="NA" customHeight="1">
-      <c r="A44" s="2" t="s">
+      <c r="A42" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B44" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D44" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E44" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F44" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G44" s="7" t="n">
-        <v>-0.03</v>
-      </c>
-      <c r="H44" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="I44" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="45" ht="NA" customHeight="1">
-      <c r="A45" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G45" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="H45" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="I45" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="46" ht="NA" customHeight="1">
-      <c r="A46" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D46" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E46" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F46" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G46" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="H46" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="I46" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="47" ht="NA" customHeight="1">
-      <c r="A47" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B47" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D47" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E47" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G47" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="H47" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="I47" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="48" ht="NA" customHeight="1">
-      <c r="A48" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B48" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C48" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D48" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E48" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F48" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G48" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="H48" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="I48" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="49" ht="NA" customHeight="1">
-      <c r="A49" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B49" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D49" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E49" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G49" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="H49" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="I49" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="50" ht="NA" customHeight="1">
-      <c r="A50" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B50" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D50" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E50" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F50" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G50" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="H50" s="7" t="n">
-        <v>-0.01</v>
-      </c>
-      <c r="I50" s="7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" ht="NA" customHeight="1">
-      <c r="A51" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B51" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E51" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F51" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G51" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="H51" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="I51" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="52" ht="NA" customHeight="1">
-      <c r="A52" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B52" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C52" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D52" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E52" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F52" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G52" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="H52" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="I52" s="7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="53" ht="NA" customHeight="1">
-      <c r="A53" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B53" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C53" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D53" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E53" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F53" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G53" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="H53" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="I53" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="54" ht="NA" customHeight="1">
-      <c r="A54" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B54" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C54" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D54" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E54" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F54" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G54" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="H54" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="I54" s="7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="55" ht="NA" customHeight="1">
-      <c r="A55" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B55" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C55" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D55" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E55" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="F55" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="G55" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="H55" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="I55" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="56" ht="NA" customHeight="1">
-      <c r="A56" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B56" s="9" t="n">
-        <v>47330</v>
-      </c>
-      <c r="C56" s="9" t="n">
-        <v>47330</v>
-      </c>
-      <c r="D56" s="9" t="n">
-        <v>47330</v>
-      </c>
-      <c r="E56" s="9" t="n">
-        <v>47330</v>
-      </c>
-      <c r="F56" s="9" t="n">
-        <v>47330</v>
-      </c>
-      <c r="G56" s="9" t="n">
-        <v>47330</v>
-      </c>
-      <c r="H56" s="9" t="n">
-        <v>47330</v>
-      </c>
-      <c r="I56" s="9" t="n">
-        <v>45146</v>
-      </c>
-    </row>
-    <row r="57" ht="NA" customHeight="1">
-      <c r="A57" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B57" s="10" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="C57" s="10" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="D57" s="10" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="E57" s="10" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="F57" s="10" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="G57" s="10" t="n">
-        <v>0.12</v>
-      </c>
-      <c r="H57" s="10" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="I57" s="10" t="n">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="58" ht="NA" customHeight="1">
-      <c r="A58" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D58" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E58" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F58" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G58" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H58" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I58" s="4" t="s">
-        <v>30</v>
+      <c r="B42" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I42" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A58:I58"/>
+    <mergeCell ref="A42:I42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
change definition of child_age var and adjust reg models
</commit_message>
<xml_diff>
--- a/OUTPUT/DATA/Regression output 2022.xlsx
+++ b/OUTPUT/DATA/Regression output 2022.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
   <si>
     <t xml:space="preserve"/>
   </si>
@@ -80,12 +80,18 @@
     <t xml:space="preserve">RELIG11_labelAny Other Religion</t>
   </si>
   <si>
-    <t xml:space="preserve">LIMITK_labelYes</t>
+    <t xml:space="preserve">DISEA_labelEquality Act Disabled</t>
   </si>
   <si>
     <t xml:space="preserve">num_children</t>
   </si>
   <si>
+    <t xml:space="preserve">parent:manchester_resident</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parent:birmingham_resident</t>
+  </si>
+  <si>
     <t xml:space="preserve">N</t>
   </si>
   <si>
@@ -221,22 +227,67 @@
     <t xml:space="preserve">-0.32 ***</t>
   </si>
   <si>
-    <t xml:space="preserve">** + health</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.79 ***</t>
+    <t xml:space="preserve">** + disability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.76 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.24 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">** + num_children</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.21 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">full</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.89 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.05 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.05 *  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.54 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.18 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.03 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.03 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.13 ** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.11 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.28 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.10 *  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.07 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">full + regions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.27 ***</t>
   </si>
   <si>
     <t xml:space="preserve">(0.04)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.35 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">** + num_children</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.21 ***</t>
   </si>
 </sst>
 </file>
@@ -704,6 +755,8 @@
     <col min="10" max="10" width="10.71" hidden="0" customWidth="1"/>
     <col min="11" max="11" width="10.71" hidden="0" customWidth="1"/>
     <col min="12" max="12" width="10.71" hidden="0" customWidth="1"/>
+    <col min="13" max="13" width="10.71" hidden="0" customWidth="1"/>
+    <col min="14" max="14" width="10.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="NA" customHeight="1">
@@ -711,37 +764,43 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="2" ht="NA" customHeight="1">
@@ -749,37 +808,43 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>28</v>
+        <v>30</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="3" ht="NA" customHeight="1">
@@ -787,37 +852,43 @@
         <v>0</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="7" t="s">
-        <v>29</v>
-      </c>
       <c r="H3" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>31</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="4" ht="NA" customHeight="1">
@@ -825,37 +896,43 @@
         <v>2</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>74</v>
+        <v>75</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="5" ht="NA" customHeight="1">
@@ -863,37 +940,43 @@
         <v>0</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="6" ht="NA" customHeight="1">
@@ -901,22 +984,22 @@
         <v>3</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D6" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F6" s="7" t="n">
         <v>-0.01</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H6" s="7" t="n">
         <v>0</v>
@@ -933,43 +1016,55 @@
       <c r="L6" s="7" t="n">
         <v>0.01</v>
       </c>
+      <c r="M6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" s="7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" ht="NA" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>67</v>
+        <v>33</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="8" ht="NA" customHeight="1">
@@ -977,37 +1072,43 @@
         <v>4</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="K8" s="7" t="n">
-        <v>-0.04</v>
+        <v>66</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>55</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="N8" s="7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="9" ht="NA" customHeight="1">
@@ -1015,37 +1116,43 @@
         <v>0</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="N9" s="7" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="10" ht="NA" customHeight="1">
@@ -1053,37 +1160,43 @@
         <v>5</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E10" s="7" t="n">
         <v>-0.03</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N10" s="7" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="11" ht="NA" customHeight="1">
@@ -1091,37 +1204,43 @@
         <v>0</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="M11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N11" s="7" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="12" ht="NA" customHeight="1">
@@ -1129,37 +1248,43 @@
         <v>6</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="M12" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N12" s="7" t="n">
+        <v>-0.02</v>
       </c>
     </row>
     <row r="13" ht="NA" customHeight="1">
@@ -1167,37 +1292,43 @@
         <v>0</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="M13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N13" s="7" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="14" ht="NA" customHeight="1">
@@ -1205,37 +1336,43 @@
         <v>7</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K14" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="M14" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="N14" s="7" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="15" ht="NA" customHeight="1">
@@ -1243,37 +1380,43 @@
         <v>0</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="M15" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="N15" s="7" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="16" ht="NA" customHeight="1">
@@ -1281,37 +1424,43 @@
         <v>8</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K16" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L16" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="M16" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="N16" s="7" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="17" ht="NA" customHeight="1">
@@ -1319,37 +1468,43 @@
         <v>0</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L17" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="M17" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="N17" s="7" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="18" ht="NA" customHeight="1">
@@ -1357,37 +1512,43 @@
         <v>9</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K18" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L18" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="M18" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="N18" s="7" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="19" ht="NA" customHeight="1">
@@ -1395,37 +1556,43 @@
         <v>0</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K19" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="M19" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="N19" s="7" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="20" ht="NA" customHeight="1">
@@ -1433,37 +1600,43 @@
         <v>10</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K20" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L20" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="M20" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="N20" s="7" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="21" ht="NA" customHeight="1">
@@ -1471,37 +1644,43 @@
         <v>0</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K21" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L21" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="M21" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="N21" s="7" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="22" ht="NA" customHeight="1">
@@ -1509,37 +1688,43 @@
         <v>11</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K22" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L22" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="M22" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N22" s="7" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="23" ht="NA" customHeight="1">
@@ -1547,37 +1732,43 @@
         <v>0</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K23" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L23" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="M23" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N23" s="7" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="24" ht="NA" customHeight="1">
@@ -1585,37 +1776,43 @@
         <v>12</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H24" s="7" t="n">
         <v>0</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K24" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L24" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="M24" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N24" s="7" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="25" ht="NA" customHeight="1">
@@ -1623,37 +1820,43 @@
         <v>0</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K25" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L25" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="M25" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N25" s="7" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="26" ht="NA" customHeight="1">
@@ -1661,37 +1864,43 @@
         <v>13</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K26" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L26" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="M26" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N26" s="7" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="27" ht="NA" customHeight="1">
@@ -1699,37 +1908,43 @@
         <v>0</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K27" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L27" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="M27" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N27" s="7" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="28" ht="NA" customHeight="1">
@@ -1737,37 +1952,43 @@
         <v>14</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K28" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L28" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="M28" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="N28" s="7" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="29" ht="NA" customHeight="1">
@@ -1775,37 +1996,43 @@
         <v>0</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K29" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L29" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="M29" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="N29" s="7" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="30" ht="NA" customHeight="1">
@@ -1813,37 +2040,43 @@
         <v>15</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="K30" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L30" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="M30" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="N30" s="7" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="31" ht="NA" customHeight="1">
@@ -1851,37 +2084,43 @@
         <v>0</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="K31" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L31" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="M31" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="N31" s="7" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="32" ht="NA" customHeight="1">
@@ -1889,37 +2128,43 @@
         <v>16</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J32" s="7" t="n">
         <v>-0.09</v>
       </c>
       <c r="K32" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L32" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="M32" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="N32" s="7" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="33" ht="NA" customHeight="1">
@@ -1927,37 +2172,43 @@
         <v>0</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J33" s="7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="K33" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L33" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="M33" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="N33" s="7" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="34" ht="NA" customHeight="1">
@@ -1965,37 +2216,43 @@
         <v>17</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J34" s="7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K34" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L34" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="M34" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="N34" s="7" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="35" ht="NA" customHeight="1">
@@ -2003,37 +2260,43 @@
         <v>0</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J35" s="7" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="K35" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L35" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="M35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="N35" s="7" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="36" ht="NA" customHeight="1">
@@ -2041,37 +2304,43 @@
         <v>18</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J36" s="7" t="n">
         <v>0.02</v>
       </c>
       <c r="K36" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L36" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="M36" s="7" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="N36" s="7" t="n">
+        <v>0.03</v>
       </c>
     </row>
     <row r="37" ht="NA" customHeight="1">
@@ -2079,37 +2348,43 @@
         <v>0</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J37" s="7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="K37" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L37" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="M37" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="N37" s="7" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="38" ht="NA" customHeight="1">
@@ -2117,37 +2392,43 @@
         <v>19</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I38" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J38" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="K38" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L38" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="M38" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="N38" s="7" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="39" ht="NA" customHeight="1">
@@ -2155,37 +2436,43 @@
         <v>0</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J39" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="K39" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L39" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="M39" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="N39" s="7" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="40" ht="NA" customHeight="1">
@@ -2193,37 +2480,43 @@
         <v>20</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I40" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J40" s="7" t="n">
         <v>-0.08</v>
       </c>
       <c r="K40" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L40" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="M40" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="N40" s="7" t="n">
+        <v>-0.09</v>
       </c>
     </row>
     <row r="41" ht="NA" customHeight="1">
@@ -2231,37 +2524,43 @@
         <v>0</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J41" s="7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="K41" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L41" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="M41" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="N41" s="7" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="42" ht="NA" customHeight="1">
@@ -2269,37 +2568,43 @@
         <v>21</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I42" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J42" s="7" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="K42" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L42" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="M42" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="N42" s="7" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="43" ht="NA" customHeight="1">
@@ -2307,37 +2612,43 @@
         <v>0</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J43" s="7" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="K43" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L43" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="M43" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="N43" s="7" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="44" ht="NA" customHeight="1">
@@ -2345,37 +2656,43 @@
         <v>22</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H44" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I44" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J44" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K44" s="7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="L44" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="M44" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N44" s="7" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="45" ht="NA" customHeight="1">
@@ -2383,37 +2700,43 @@
         <v>0</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J45" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K45" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="L45" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="M45" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="N45" s="7" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="46" ht="NA" customHeight="1">
@@ -2421,194 +2744,400 @@
         <v>23</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H46" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I46" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J46" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K46" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L46" s="7" t="s">
-        <v>60</v>
+        <v>62</v>
+      </c>
+      <c r="M46" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="N46" s="7" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="47" ht="NA" customHeight="1">
       <c r="A47" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B47" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C47" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D47" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E47" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F47" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G47" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="H47" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="I47" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="J47" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="K47" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="L47" s="8" t="s">
-        <v>31</v>
+      <c r="B47" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G47" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H47" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I47" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J47" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="K47" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="L47" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="M47" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="N47" s="7" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="48" ht="NA" customHeight="1">
       <c r="A48" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B48" s="9" t="n">
+      <c r="B48" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H48" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I48" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J48" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="K48" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="L48" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="M48" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N48" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" ht="NA" customHeight="1">
+      <c r="A49" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F49" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G49" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H49" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I49" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J49" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="K49" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="L49" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="M49" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N49" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="50" ht="NA" customHeight="1">
+      <c r="A50" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G50" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H50" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I50" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J50" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="K50" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="L50" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="M50" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N50" s="7" t="n">
+        <v>-0.07</v>
+      </c>
+    </row>
+    <row r="51" ht="NA" customHeight="1">
+      <c r="A51" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E51" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G51" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H51" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I51" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="J51" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="K51" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="L51" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="M51" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="N51" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="52" ht="NA" customHeight="1">
+      <c r="A52" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B52" s="9" t="n">
         <v>24675</v>
       </c>
-      <c r="C48" s="9" t="n">
+      <c r="C52" s="9" t="n">
         <v>24675</v>
       </c>
-      <c r="D48" s="9" t="n">
+      <c r="D52" s="9" t="n">
         <v>24675</v>
       </c>
-      <c r="E48" s="9" t="n">
+      <c r="E52" s="9" t="n">
         <v>24675</v>
       </c>
-      <c r="F48" s="9" t="n">
+      <c r="F52" s="9" t="n">
         <v>24675</v>
       </c>
-      <c r="G48" s="9" t="n">
+      <c r="G52" s="9" t="n">
         <v>23680</v>
       </c>
-      <c r="H48" s="9" t="n">
+      <c r="H52" s="9" t="n">
         <v>24675</v>
       </c>
-      <c r="I48" s="9" t="n">
+      <c r="I52" s="9" t="n">
         <v>24675</v>
       </c>
-      <c r="J48" s="9" t="n">
+      <c r="J52" s="9" t="n">
         <v>21425</v>
       </c>
-      <c r="K48" s="9" t="n">
-        <v>8910</v>
-      </c>
-      <c r="L48" s="9" t="n">
+      <c r="K52" s="9" t="n">
+        <v>24479</v>
+      </c>
+      <c r="L52" s="9" t="n">
         <v>24675</v>
       </c>
-    </row>
-    <row r="49" ht="NA" customHeight="1">
-      <c r="A49" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B49" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="C49" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="D49" s="10" t="n">
+      <c r="M52" s="9" t="n">
+        <v>21281</v>
+      </c>
+      <c r="N52" s="9" t="n">
+        <v>21281</v>
+      </c>
+    </row>
+    <row r="53" ht="NA" customHeight="1">
+      <c r="A53" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B53" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C53" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D53" s="10" t="n">
         <v>0.01</v>
       </c>
-      <c r="E49" s="10" t="n">
+      <c r="E53" s="10" t="n">
         <v>0.01</v>
       </c>
-      <c r="F49" s="10" t="n">
+      <c r="F53" s="10" t="n">
         <v>0.07</v>
       </c>
-      <c r="G49" s="10" t="n">
+      <c r="G53" s="10" t="n">
         <v>0.02</v>
       </c>
-      <c r="H49" s="10" t="n">
+      <c r="H53" s="10" t="n">
         <v>0.01</v>
       </c>
-      <c r="I49" s="10" t="n">
+      <c r="I53" s="10" t="n">
         <v>0.01</v>
       </c>
-      <c r="J49" s="10" t="n">
+      <c r="J53" s="10" t="n">
         <v>0.03</v>
       </c>
-      <c r="K49" s="10" t="n">
-        <v>0.13</v>
-      </c>
-      <c r="L49" s="10" t="n">
+      <c r="K53" s="10" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="L53" s="10" t="n">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="50" ht="NA" customHeight="1">
-      <c r="A50" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E50" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F50" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G50" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H50" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I50" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J50" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K50" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="L50" s="4" t="s">
-        <v>26</v>
+      <c r="M53" s="10" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="N53" s="10" t="n">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="54" ht="NA" customHeight="1">
+      <c r="A54" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G54" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H54" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I54" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J54" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K54" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L54" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M54" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N54" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A50:L50"/>
+    <mergeCell ref="A54:N54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
create function for regressions
</commit_message>
<xml_diff>
--- a/OUTPUT/DATA/Regression output 2022.xlsx
+++ b/OUTPUT/DATA/Regression output 2022.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="122">
   <si>
     <t xml:space="preserve"/>
   </si>
@@ -86,142 +86,305 @@
     <t xml:space="preserve">Main simple (**)</t>
   </si>
   <si>
-    <t xml:space="preserve">0.77 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.01)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.07 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.02)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">       </t>
+    <t xml:space="preserve">0.7663 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.005635)  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.07325 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.01821)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">          </t>
   </si>
   <si>
     <t xml:space="preserve">** + age</t>
   </si>
   <si>
-    <t xml:space="preserve">0.70 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.09 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.66 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.03)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.18 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.05)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.11 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.08 ***</t>
+    <t xml:space="preserve">0.6982 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0122)    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.08508 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.01801)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.6564 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.03344)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.1826 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.05439)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1088 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.01387)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.08431 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.01802)   </t>
   </si>
   <si>
     <t xml:space="preserve">** + eth</t>
   </si>
   <si>
-    <t xml:space="preserve">0.79 ***</t>
+    <t xml:space="preserve">0.7929 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.005796) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0189)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.1776 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.01639)  </t>
   </si>
   <si>
     <t xml:space="preserve">** + child age</t>
   </si>
   <si>
-    <t xml:space="preserve">0.80 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.08 ***</t>
+    <t xml:space="preserve">0.7982 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.006492)  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.07134 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.018)     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.08059 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.01389)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.08347 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.01686)   </t>
   </si>
   <si>
     <t xml:space="preserve">** + famtype</t>
   </si>
   <si>
-    <t xml:space="preserve">0.66 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.13 ***</t>
+    <t xml:space="preserve">0.6606 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.01302)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.07699 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.01817)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1333 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.01418)   </t>
   </si>
   <si>
     <t xml:space="preserve">** + religion</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.04 *  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.17 *  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.07)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.04)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.34 ***</t>
+    <t xml:space="preserve">0.7869 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.008095) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.03682 * </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.01859)  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.01136)  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.1687 *  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.07199)  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.03996)  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.06598)  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.3424 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.02688)  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.06955)  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.05128)  </t>
   </si>
   <si>
     <t xml:space="preserve">** + disability</t>
   </si>
   <si>
-    <t xml:space="preserve">0.82 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.25 ***</t>
+    <t xml:space="preserve">0.8211 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.005834)  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.08622 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.01795)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.2489 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.01452)   </t>
   </si>
   <si>
     <t xml:space="preserve">** + num_children</t>
   </si>
   <si>
-    <t xml:space="preserve">0.87 ***</t>
+    <t xml:space="preserve">0.8739 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.01081)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.07151 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.01775)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.06889 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.00638)   </t>
   </si>
   <si>
     <t xml:space="preserve">full</t>
   </si>
   <si>
-    <t xml:space="preserve">0.85 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.74 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.09 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.18 *  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.06)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.26 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.08)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.23 ***</t>
+    <t xml:space="preserve">0.8451 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.01921)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.04322 *  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.01785)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.7437 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.02845)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.1767 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.05087)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.09348 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.01355)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0186)    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.07781 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.02036)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.09235 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.01392)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.01088)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.1803 *   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.07338)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.04266)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.05827)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.2611 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.03166)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.07542)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.04665)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.2252 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.01474)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.07183 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.006596)  </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
-    <numFmt numFmtId="166" formatCode="0.00"/>
-    <numFmt numFmtId="167" formatCode="0.00"/>
-    <numFmt numFmtId="168" formatCode="0.00"/>
-    <numFmt numFmtId="169" formatCode="0.00"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -340,7 +503,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="0" horizontal="center" vertical="top" wrapText="1"/>
@@ -357,19 +520,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="0" horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="0" horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="0" horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="0" horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="0" horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="0" horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="0" horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="0" horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -688,25 +848,25 @@
         <v>29</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>57</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" ht="NA" customHeight="1">
@@ -720,25 +880,25 @@
         <v>30</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>53</v>
+        <v>80</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>56</v>
+        <v>87</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>58</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" ht="NA" customHeight="1">
@@ -749,28 +909,28 @@
         <v>25</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>25</v>
+        <v>88</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>27</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" ht="NA" customHeight="1">
@@ -781,28 +941,28 @@
         <v>26</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D4" s="7" t="n">
-        <v>-0.03</v>
+        <v>-0.03046</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>31</v>
+        <v>82</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>26</v>
+        <v>89</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>47</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" ht="NA" customHeight="1">
@@ -813,28 +973,28 @@
         <v>27</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>27</v>
+        <v>83</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>27</v>
+        <v>90</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>27</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" ht="NA" customHeight="1">
@@ -845,10 +1005,10 @@
         <v>28</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>28</v>
@@ -857,7 +1017,7 @@
         <v>28</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>28</v>
@@ -866,7 +1026,7 @@
         <v>28</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>59</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" ht="NA" customHeight="1">
@@ -877,10 +1037,10 @@
         <v>28</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>28</v>
@@ -889,7 +1049,7 @@
         <v>28</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>28</v>
@@ -898,7 +1058,7 @@
         <v>28</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" ht="NA" customHeight="1">
@@ -909,10 +1069,10 @@
         <v>28</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>28</v>
@@ -921,7 +1081,7 @@
         <v>28</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>28</v>
@@ -930,7 +1090,7 @@
         <v>28</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>34</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" ht="NA" customHeight="1">
@@ -941,10 +1101,10 @@
         <v>28</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>28</v>
@@ -953,7 +1113,7 @@
         <v>28</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>28</v>
@@ -962,7 +1122,7 @@
         <v>28</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>35</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" ht="NA" customHeight="1">
@@ -973,10 +1133,10 @@
         <v>28</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>28</v>
@@ -985,7 +1145,7 @@
         <v>28</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="H10" s="7" t="s">
         <v>28</v>
@@ -994,7 +1154,7 @@
         <v>28</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>60</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" ht="NA" customHeight="1">
@@ -1005,10 +1165,10 @@
         <v>28</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>28</v>
@@ -1017,7 +1177,7 @@
         <v>28</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="H11" s="7" t="s">
         <v>28</v>
@@ -1026,7 +1186,7 @@
         <v>28</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>25</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" ht="NA" customHeight="1">
@@ -1037,10 +1197,10 @@
         <v>28</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>28</v>
@@ -1049,7 +1209,7 @@
         <v>28</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="H12" s="7" t="s">
         <v>28</v>
@@ -1058,7 +1218,7 @@
         <v>28</v>
       </c>
       <c r="J12" s="7" t="n">
-        <v>0</v>
+        <v>-0.003412</v>
       </c>
     </row>
     <row r="13" ht="NA" customHeight="1">
@@ -1069,10 +1229,10 @@
         <v>28</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>28</v>
@@ -1081,7 +1241,7 @@
         <v>28</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>28</v>
@@ -1090,7 +1250,7 @@
         <v>28</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>27</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" ht="NA" customHeight="1">
@@ -1104,7 +1264,7 @@
         <v>28</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>28</v>
@@ -1113,7 +1273,7 @@
         <v>28</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="H14" s="7" t="s">
         <v>28</v>
@@ -1122,7 +1282,7 @@
         <v>28</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>42</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" ht="NA" customHeight="1">
@@ -1136,7 +1296,7 @@
         <v>28</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>28</v>
@@ -1145,7 +1305,7 @@
         <v>28</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>28</v>
@@ -1154,7 +1314,7 @@
         <v>28</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>27</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" ht="NA" customHeight="1">
@@ -1168,16 +1328,16 @@
         <v>28</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>28</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="H16" s="7" t="s">
         <v>28</v>
@@ -1200,16 +1360,16 @@
         <v>28</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="F17" s="7" t="s">
         <v>28</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="H17" s="7" t="s">
         <v>28</v>
@@ -1232,16 +1392,16 @@
         <v>28</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="F18" s="7" t="s">
         <v>28</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>28</v>
@@ -1264,16 +1424,16 @@
         <v>28</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="F19" s="7" t="s">
         <v>28</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="H19" s="7" t="s">
         <v>28</v>
@@ -1296,16 +1456,16 @@
         <v>28</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>28</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="H20" s="7" t="s">
         <v>28</v>
@@ -1314,7 +1474,7 @@
         <v>28</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>60</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21" ht="NA" customHeight="1">
@@ -1328,16 +1488,16 @@
         <v>28</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>28</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="H21" s="7" t="s">
         <v>28</v>
@@ -1346,7 +1506,7 @@
         <v>28</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>25</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22" ht="NA" customHeight="1">
@@ -1360,7 +1520,7 @@
         <v>28</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>28</v>
@@ -1369,7 +1529,7 @@
         <v>28</v>
       </c>
       <c r="G22" s="7" t="n">
-        <v>0.01</v>
+        <v>0.005326</v>
       </c>
       <c r="H22" s="7" t="s">
         <v>28</v>
@@ -1378,7 +1538,7 @@
         <v>28</v>
       </c>
       <c r="J22" s="7" t="n">
-        <v>-0.02</v>
+        <v>-0.01708</v>
       </c>
     </row>
     <row r="23" ht="NA" customHeight="1">
@@ -1392,7 +1552,7 @@
         <v>28</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>28</v>
@@ -1401,7 +1561,7 @@
         <v>28</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="H23" s="7" t="s">
         <v>28</v>
@@ -1410,7 +1570,7 @@
         <v>28</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>25</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24" ht="NA" customHeight="1">
@@ -1424,7 +1584,7 @@
         <v>28</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>28</v>
@@ -1433,7 +1593,7 @@
         <v>28</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="H24" s="7" t="s">
         <v>28</v>
@@ -1442,7 +1602,7 @@
         <v>28</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>61</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25" ht="NA" customHeight="1">
@@ -1456,7 +1616,7 @@
         <v>28</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>28</v>
@@ -1465,7 +1625,7 @@
         <v>28</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="H25" s="7" t="s">
         <v>28</v>
@@ -1474,7 +1634,7 @@
         <v>28</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>49</v>
+        <v>111</v>
       </c>
     </row>
     <row r="26" ht="NA" customHeight="1">
@@ -1488,7 +1648,7 @@
         <v>28</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>28</v>
@@ -1497,7 +1657,7 @@
         <v>28</v>
       </c>
       <c r="G26" s="7" t="n">
-        <v>-0.03</v>
+        <v>-0.03239</v>
       </c>
       <c r="H26" s="7" t="s">
         <v>28</v>
@@ -1506,7 +1666,7 @@
         <v>28</v>
       </c>
       <c r="J26" s="7" t="n">
-        <v>-0.04</v>
+        <v>-0.0391</v>
       </c>
     </row>
     <row r="27" ht="NA" customHeight="1">
@@ -1520,7 +1680,7 @@
         <v>28</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>28</v>
@@ -1529,7 +1689,7 @@
         <v>28</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="H27" s="7" t="s">
         <v>28</v>
@@ -1538,7 +1698,7 @@
         <v>28</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>50</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28" ht="NA" customHeight="1">
@@ -1552,7 +1712,7 @@
         <v>28</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>28</v>
@@ -1561,7 +1721,7 @@
         <v>28</v>
       </c>
       <c r="G28" s="7" t="n">
-        <v>0.07</v>
+        <v>0.07349</v>
       </c>
       <c r="H28" s="7" t="s">
         <v>28</v>
@@ -1570,7 +1730,7 @@
         <v>28</v>
       </c>
       <c r="J28" s="7" t="n">
-        <v>0.07</v>
+        <v>0.06587</v>
       </c>
     </row>
     <row r="29" ht="NA" customHeight="1">
@@ -1584,7 +1744,7 @@
         <v>28</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>28</v>
@@ -1593,7 +1753,7 @@
         <v>28</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="H29" s="7" t="s">
         <v>28</v>
@@ -1602,7 +1762,7 @@
         <v>28</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>62</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" ht="NA" customHeight="1">
@@ -1616,7 +1776,7 @@
         <v>28</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>28</v>
@@ -1625,7 +1785,7 @@
         <v>28</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="H30" s="7" t="s">
         <v>28</v>
@@ -1634,7 +1794,7 @@
         <v>28</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>63</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" ht="NA" customHeight="1">
@@ -1648,7 +1808,7 @@
         <v>28</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>28</v>
@@ -1657,7 +1817,7 @@
         <v>28</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="H31" s="7" t="s">
         <v>28</v>
@@ -1666,7 +1826,7 @@
         <v>28</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>33</v>
+        <v>115</v>
       </c>
     </row>
     <row r="32" ht="NA" customHeight="1">
@@ -1680,7 +1840,7 @@
         <v>28</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="E32" s="7" t="s">
         <v>28</v>
@@ -1689,7 +1849,7 @@
         <v>28</v>
       </c>
       <c r="G32" s="7" t="n">
-        <v>-0.09</v>
+        <v>-0.0885</v>
       </c>
       <c r="H32" s="7" t="s">
         <v>28</v>
@@ -1698,7 +1858,7 @@
         <v>28</v>
       </c>
       <c r="J32" s="7" t="n">
-        <v>-0.07</v>
+        <v>-0.0726</v>
       </c>
     </row>
     <row r="33" ht="NA" customHeight="1">
@@ -1712,7 +1872,7 @@
         <v>28</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="E33" s="7" t="s">
         <v>28</v>
@@ -1721,7 +1881,7 @@
         <v>28</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="H33" s="7" t="s">
         <v>28</v>
@@ -1730,7 +1890,7 @@
         <v>28</v>
       </c>
       <c r="J33" s="7" t="s">
-        <v>64</v>
+        <v>116</v>
       </c>
     </row>
     <row r="34" ht="NA" customHeight="1">
@@ -1744,7 +1904,7 @@
         <v>28</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>28</v>
@@ -1753,7 +1913,7 @@
         <v>28</v>
       </c>
       <c r="G34" s="7" t="n">
-        <v>-0.09</v>
+        <v>-0.09389</v>
       </c>
       <c r="H34" s="7" t="s">
         <v>28</v>
@@ -1762,7 +1922,7 @@
         <v>28</v>
       </c>
       <c r="J34" s="7" t="n">
-        <v>-0.08</v>
+        <v>-0.07568</v>
       </c>
     </row>
     <row r="35" ht="NA" customHeight="1">
@@ -1776,7 +1936,7 @@
         <v>28</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>28</v>
@@ -1785,7 +1945,7 @@
         <v>28</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>35</v>
+        <v>78</v>
       </c>
       <c r="H35" s="7" t="s">
         <v>28</v>
@@ -1794,7 +1954,7 @@
         <v>28</v>
       </c>
       <c r="J35" s="7" t="s">
-        <v>35</v>
+        <v>117</v>
       </c>
     </row>
     <row r="36" ht="NA" customHeight="1">
@@ -1808,7 +1968,7 @@
         <v>28</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="E36" s="7" t="s">
         <v>28</v>
@@ -1817,16 +1977,16 @@
         <v>28</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>54</v>
+        <v>84</v>
       </c>
       <c r="I36" s="7" t="s">
         <v>28</v>
       </c>
       <c r="J36" s="7" t="s">
-        <v>65</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37" ht="NA" customHeight="1">
@@ -1840,7 +2000,7 @@
         <v>28</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>28</v>
@@ -1849,16 +2009,16 @@
         <v>28</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>25</v>
+        <v>85</v>
       </c>
       <c r="I37" s="7" t="s">
         <v>28</v>
       </c>
       <c r="J37" s="7" t="s">
-        <v>25</v>
+        <v>119</v>
       </c>
     </row>
     <row r="38" ht="NA" customHeight="1">
@@ -1872,7 +2032,7 @@
         <v>28</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="E38" s="7" t="s">
         <v>28</v>
@@ -1881,16 +2041,16 @@
         <v>28</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="H38" s="7" t="s">
         <v>28</v>
       </c>
       <c r="I38" s="7" t="s">
-        <v>26</v>
+        <v>91</v>
       </c>
       <c r="J38" s="7" t="s">
-        <v>26</v>
+        <v>120</v>
       </c>
     </row>
     <row r="39" ht="NA" customHeight="1">
@@ -1904,7 +2064,7 @@
         <v>28</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="E39" s="8" t="s">
         <v>28</v>
@@ -1913,47 +2073,47 @@
         <v>28</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="H39" s="8" t="s">
         <v>28</v>
       </c>
       <c r="I39" s="8" t="s">
-        <v>25</v>
+        <v>92</v>
       </c>
       <c r="J39" s="8" t="s">
-        <v>25</v>
+        <v>121</v>
       </c>
     </row>
     <row r="40" ht="NA" customHeight="1">
       <c r="A40" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B40" s="9" t="n">
+      <c r="B40" s="6" t="n">
         <v>8685</v>
       </c>
-      <c r="C40" s="9" t="n">
+      <c r="C40" s="6" t="n">
         <v>8685</v>
       </c>
-      <c r="D40" s="9" t="n">
+      <c r="D40" s="6" t="n">
         <v>8468</v>
       </c>
-      <c r="E40" s="9" t="n">
+      <c r="E40" s="6" t="n">
         <v>8685</v>
       </c>
-      <c r="F40" s="9" t="n">
+      <c r="F40" s="6" t="n">
         <v>8685</v>
       </c>
-      <c r="G40" s="9" t="n">
+      <c r="G40" s="6" t="n">
         <v>7611</v>
       </c>
-      <c r="H40" s="9" t="n">
+      <c r="H40" s="6" t="n">
         <v>8626</v>
       </c>
-      <c r="I40" s="9" t="n">
+      <c r="I40" s="6" t="n">
         <v>8685</v>
       </c>
-      <c r="J40" s="9" t="n">
+      <c r="J40" s="6" t="n">
         <v>7567</v>
       </c>
     </row>
@@ -1961,32 +2121,32 @@
       <c r="A41" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B41" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="C41" s="10" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="D41" s="10" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="E41" s="10" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="F41" s="10" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="G41" s="10" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="H41" s="10" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="I41" s="10" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="J41" s="10" t="n">
-        <v>0.15</v>
+      <c r="B41" s="9" t="n">
+        <v>0.003612</v>
+      </c>
+      <c r="C41" s="9" t="n">
+        <v>0.02556</v>
+      </c>
+      <c r="D41" s="9" t="n">
+        <v>0.02967</v>
+      </c>
+      <c r="E41" s="9" t="n">
+        <v>0.01223</v>
+      </c>
+      <c r="F41" s="9" t="n">
+        <v>0.01919</v>
+      </c>
+      <c r="G41" s="9" t="n">
+        <v>0.05098</v>
+      </c>
+      <c r="H41" s="9" t="n">
+        <v>0.05886</v>
+      </c>
+      <c r="I41" s="9" t="n">
+        <v>0.02571</v>
+      </c>
+      <c r="J41" s="9" t="n">
+        <v>0.1525</v>
       </c>
     </row>
     <row r="42" ht="NA" customHeight="1">

</xml_diff>

<commit_message>
add outputs from network drive to main project; add level of quals to code
</commit_message>
<xml_diff>
--- a/OUTPUT/DATA/Regression output 2022.xlsx
+++ b/OUTPUT/DATA/Regression output 2022.xlsx
@@ -1,37 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://greaterlondonauthority.sharepoint.com/sites/S_IU_GLAEconomics/Shared Documents/General/Micro/Labour Market/Ad hoc work/12. Childcare and employment/R/OUTPUT/DATA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{8CF2445D-7569-4169-BD10-D72C3B122BFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17B1A09F-8618-48B7-85B1-F3D689E73BA1}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_CDD63AD52F15F1A701088A6B4B8CE1BA258B71EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5FADB71C-84D3-4305-9940-C0CDA18B6450}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="153">
   <si>
     <t/>
   </si>
@@ -93,6 +82,24 @@
     <t>num_children</t>
   </si>
   <si>
+    <t>lev_quals_labelDegree or Equivalent</t>
+  </si>
+  <si>
+    <t>lev_quals_labelHigher Education</t>
+  </si>
+  <si>
+    <t>lev_quals_labelGCE A Level or Equivalent</t>
+  </si>
+  <si>
+    <t>lev_quals_labelGCSE Grades A*-C or Equivalent</t>
+  </si>
+  <si>
+    <t>lev_quals_labelOther Qualifications</t>
+  </si>
+  <si>
+    <t>lev_quals_labelDK</t>
+  </si>
+  <si>
     <t>N</t>
   </si>
   <si>
@@ -105,292 +112,373 @@
     <t>Main simple (**)</t>
   </si>
   <si>
-    <t xml:space="preserve">0.7663 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.005635)  </t>
-  </si>
-  <si>
-    <t>-0.07325 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.01821)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">          </t>
+    <t xml:space="preserve">0.766 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.00564)  </t>
+  </si>
+  <si>
+    <t>-0.0733 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0182)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         </t>
   </si>
   <si>
     <t>** + age</t>
   </si>
   <si>
-    <t xml:space="preserve">0.6982 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0122)    </t>
-  </si>
-  <si>
-    <t>-0.08508 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.01801)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.6564 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.03344)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.1826 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.05439)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.1088 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.01387)   </t>
-  </si>
-  <si>
-    <t>0.08431 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.01802)   </t>
+    <t xml:space="preserve">0.698 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0122)   </t>
+  </si>
+  <si>
+    <t>-0.0851 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.018)    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.656 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0334)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.183 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0544)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.109 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0139)   </t>
+  </si>
+  <si>
+    <t>0.0843 ***</t>
   </si>
   <si>
     <t>** + eth</t>
   </si>
   <si>
-    <t>0.7929 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.005796) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0189)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">         </t>
-  </si>
-  <si>
-    <t>-0.1776 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.01639)  </t>
+    <t>0.793 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0058)  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0189)  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        </t>
+  </si>
+  <si>
+    <t>-0.178 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0164)  </t>
   </si>
   <si>
     <t>** + child age</t>
   </si>
   <si>
-    <t xml:space="preserve">0.7982 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.006492)  </t>
-  </si>
-  <si>
-    <t>-0.07134 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.018)     </t>
-  </si>
-  <si>
-    <t>-0.08059 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.01389)   </t>
-  </si>
-  <si>
-    <t>-0.08347 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.01686)   </t>
+    <t xml:space="preserve">0.798 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.00649)  </t>
+  </si>
+  <si>
+    <t>-0.0713 ***</t>
+  </si>
+  <si>
+    <t>-0.0806 ***</t>
+  </si>
+  <si>
+    <t>-0.0835 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0169)   </t>
   </si>
   <si>
     <t>** + famtype</t>
   </si>
   <si>
-    <t xml:space="preserve">0.6606 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.01302)   </t>
-  </si>
-  <si>
-    <t>-0.07699 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.01817)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.1333 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.01418)   </t>
+    <t>0.661 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.013)   </t>
+  </si>
+  <si>
+    <t>-0.077 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0182)  </t>
+  </si>
+  <si>
+    <t>0.133 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0142)  </t>
   </si>
   <si>
     <t>** + religion</t>
   </si>
   <si>
-    <t>0.7869 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.008095) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.03682 * </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.01859)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.01136)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.07199)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.03996)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.06598)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.02688)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.06955)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.05128)  </t>
+    <t>0.787 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0081)  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0368 * </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0186)  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0114)  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.169 *  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.072)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.04)    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.066)   </t>
+  </si>
+  <si>
+    <t>-0.342 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0269)  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0695)  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0513)  </t>
   </si>
   <si>
     <t>** + disability</t>
   </si>
   <si>
-    <t xml:space="preserve">0.8211 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.005834)  </t>
-  </si>
-  <si>
-    <t>-0.08622 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.01795)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.2489 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.01452)   </t>
+    <t xml:space="preserve">0.821 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.00583)  </t>
+  </si>
+  <si>
+    <t>-0.0862 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0179)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.249 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0145)   </t>
   </si>
   <si>
     <t>** + num_children</t>
   </si>
   <si>
-    <t xml:space="preserve">0.8739 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.01081)   </t>
-  </si>
-  <si>
-    <t>-0.07151 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.01775)   </t>
-  </si>
-  <si>
-    <t>-0.06889 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.00638)   </t>
+    <t xml:space="preserve">0.874 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0108)   </t>
+  </si>
+  <si>
+    <t>-0.0715 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0177)   </t>
+  </si>
+  <si>
+    <t>-0.0689 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.00638)  </t>
+  </si>
+  <si>
+    <t>** + lev_quals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.385 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0262)   </t>
+  </si>
+  <si>
+    <t>-0.0902 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0176)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.485 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0268)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.395 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0329)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.397 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0289)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.289 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.03)     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.269 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0358)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.346 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0494)   </t>
   </si>
   <si>
     <t>full</t>
   </si>
   <si>
-    <t xml:space="preserve">0.8451 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.01921)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.04322 *  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.01785)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.7437 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.02845)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.1767 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.05087)   </t>
-  </si>
-  <si>
-    <t>0.09348 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.01355)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0186)    </t>
-  </si>
-  <si>
-    <t>-0.07781 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.02036)   </t>
-  </si>
-  <si>
-    <t>0.09235 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.01392)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.01088)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.1803 *   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.07338)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.04266)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.05827)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.2611 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.03166)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.07542)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.04665)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.2252 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.01474)   </t>
-  </si>
-  <si>
-    <t>-0.07183 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.006596)  </t>
+    <t xml:space="preserve">0.583 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0323)   </t>
+  </si>
+  <si>
+    <t>-0.0588 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0175)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.589 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.107)    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.147 **  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0517)   </t>
+  </si>
+  <si>
+    <t>0.0789 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0133)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0181)   </t>
+  </si>
+  <si>
+    <t>-0.0736 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0199)   </t>
+  </si>
+  <si>
+    <t>0.0594 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0138)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0106)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.151 *   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0704)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0421)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.052)    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.225 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0312)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0735)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0448)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.2 ***   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0144)   </t>
+  </si>
+  <si>
+    <t>-0.0674 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.00644)  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.355 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0276)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.274 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.033)    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.294 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0292)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.219 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0297)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0354)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.259 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.048)    </t>
   </si>
 </sst>
 </file>
@@ -810,1343 +898,1911 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.86328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.1328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="11" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>96</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>97</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>98</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="D4" s="6">
-        <v>-3.0460000000000001E-2</v>
+        <v>-3.0499999999999999E-2</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>99</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>100</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="J12" s="6">
-        <v>-3.4120000000000001E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K12" s="6">
+        <v>-3.8600000000000001E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="H21" s="6"/>
+        <v>51</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="I21" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+      <c r="K21" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="G22" s="6">
-        <v>5.326E-3</v>
-      </c>
-      <c r="H22" s="6"/>
+        <v>5.3299999999999997E-3</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="I22" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="J22" s="6">
-        <v>-1.7080000000000001E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K22" s="6">
+        <v>-1.8499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="H23" s="6"/>
+        <v>73</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="I23" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+      <c r="K23" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G24" s="6">
-        <v>-0.16869999999999999</v>
-      </c>
-      <c r="H24" s="6"/>
+        <v>51</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="I24" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="H25" s="6"/>
+        <v>75</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="I25" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+      <c r="K25" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="G26" s="6">
-        <v>-3.2390000000000002E-2</v>
-      </c>
-      <c r="H26" s="6"/>
+        <v>-3.2399999999999998E-2</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="I26" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="J26" s="6">
-        <v>-3.9100000000000003E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+      <c r="J26" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K26" s="6">
+        <v>-5.5599999999999997E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="H27" s="6"/>
+        <v>76</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="I27" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+      <c r="K27" s="6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="G28" s="6">
-        <v>7.349E-2</v>
-      </c>
-      <c r="H28" s="6"/>
+        <v>7.3499999999999996E-2</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="I28" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="J28" s="6">
-        <v>6.5869999999999998E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+      <c r="J28" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K28" s="6">
+        <v>5.3699999999999998E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="H29" s="6"/>
+        <v>77</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="I29" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+      <c r="K29" s="6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G30" s="6">
-        <v>-0.34239999999999998</v>
-      </c>
-      <c r="H30" s="6"/>
+        <v>51</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="I30" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+      <c r="K30" s="6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="H31" s="6"/>
+        <v>79</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="I31" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+      <c r="K31" s="6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="G32" s="6">
         <v>-8.8499999999999995E-2</v>
       </c>
-      <c r="H32" s="6"/>
+      <c r="H32" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="I32" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="J32" s="6">
-        <v>-7.2599999999999998E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+      <c r="J32" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K32" s="6">
+        <v>-7.5700000000000003E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="H33" s="6"/>
+        <v>80</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="I33" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+      <c r="K33" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="G34" s="6">
-        <v>-9.3890000000000001E-2</v>
-      </c>
-      <c r="H34" s="6"/>
+        <v>-9.3899999999999997E-2</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="I34" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="J34" s="6">
-        <v>-7.5679999999999997E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+      <c r="J34" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K34" s="6">
+        <v>-7.8600000000000003E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="H35" s="6"/>
+        <v>81</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="I35" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+      <c r="K35" s="6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="I36" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+      <c r="K36" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="I37" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+      <c r="K37" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="I38" s="6" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="J38" s="6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+      <c r="K38" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B39" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G39" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="H39" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I39" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="J39" s="7" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B39" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H39" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I39" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="J39" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K39" s="6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B40" s="5">
+      <c r="B40" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H40" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I40" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J40" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="K40" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H41" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I41" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J41" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="K41" s="6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H42" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I42" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J42" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="K42" s="6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H43" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I43" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J43" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="K43" s="6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G44" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H44" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I44" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J44" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="K44" s="6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G45" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H45" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I45" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J45" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="K45" s="6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G46" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H46" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I46" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J46" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="K46" s="6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H47" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I47" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J47" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="K47" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G48" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H48" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I48" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J48" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="K48" s="6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G49" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H49" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I49" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J49" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="K49" s="6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G50" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H50" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I50" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J50" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="K50" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G51" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H51" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I51" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J51" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="K51" s="7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B52" s="5">
         <v>8685</v>
       </c>
-      <c r="C40" s="5">
+      <c r="C52" s="5">
         <v>8685</v>
       </c>
-      <c r="D40" s="5">
+      <c r="D52" s="5">
         <v>8468</v>
       </c>
-      <c r="E40" s="5">
+      <c r="E52" s="5">
         <v>8685</v>
       </c>
-      <c r="F40" s="5">
+      <c r="F52" s="5">
         <v>8685</v>
       </c>
-      <c r="G40" s="5">
+      <c r="G52" s="5">
         <v>7611</v>
       </c>
-      <c r="H40" s="5">
+      <c r="H52" s="5">
         <v>8626</v>
       </c>
-      <c r="I40" s="5">
+      <c r="I52" s="5">
         <v>8685</v>
       </c>
-      <c r="J40" s="5">
-        <v>7567</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B41" s="8">
-        <v>3.6120000000000002E-3</v>
-      </c>
-      <c r="C41" s="8">
-        <v>2.5559999999999999E-2</v>
-      </c>
-      <c r="D41" s="8">
-        <v>2.9669999999999998E-2</v>
-      </c>
-      <c r="E41" s="8">
-        <v>1.223E-2</v>
-      </c>
-      <c r="F41" s="8">
-        <v>1.9189999999999999E-2</v>
-      </c>
-      <c r="G41" s="8">
-        <v>5.0979999999999998E-2</v>
-      </c>
-      <c r="H41" s="8">
-        <v>5.8860000000000003E-2</v>
-      </c>
-      <c r="I41" s="8">
-        <v>2.571E-2</v>
-      </c>
-      <c r="J41" s="8">
-        <v>0.1525</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D42" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E42" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="F42" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G42" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H42" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="I42" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="J42" s="9" t="s">
-        <v>22</v>
+      <c r="J52" s="5">
+        <v>8624</v>
+      </c>
+      <c r="K52" s="5">
+        <v>7517</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B53" s="8">
+        <v>3.6099999999999999E-3</v>
+      </c>
+      <c r="C53" s="8">
+        <v>2.5600000000000001E-2</v>
+      </c>
+      <c r="D53" s="8">
+        <v>2.9700000000000001E-2</v>
+      </c>
+      <c r="E53" s="8">
+        <v>1.2200000000000001E-2</v>
+      </c>
+      <c r="F53" s="8">
+        <v>1.9199999999999998E-2</v>
+      </c>
+      <c r="G53" s="8">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="H53" s="8">
+        <v>5.8900000000000001E-2</v>
+      </c>
+      <c r="I53" s="8">
+        <v>2.5700000000000001E-2</v>
+      </c>
+      <c r="J53" s="8">
+        <v>8.7499999999999994E-2</v>
+      </c>
+      <c r="K53" s="8">
+        <v>0.193</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E54" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F54" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G54" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="H54" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I54" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J54" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="K54" s="9" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A42:J42"/>
+    <mergeCell ref="A54:K54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2406,7 +3062,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{94CEF1F5-0BEB-4F82-94B4-F71FBD6C08DD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B4EA18D-3098-4636-8ED6-FF903714B046}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
@@ -2414,7 +3070,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FAA33D9-D3D6-4681-976C-D641EB232EC6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B35D537-42A5-435B-B9C4-67CF453C5E25}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>

</xml_diff>